<commit_message>
Update 2023-24 ADS&AI Assessment Rubric Y2A.xlsx
</commit_message>
<xml_diff>
--- a/docs/Year2/BlockA/MS Teams Assignment Template/2023-24/2023-24 ADS&AI Assessment Rubric Y2A.xlsx
+++ b/docs/Year2/BlockA/MS Teams Assignment Template/2023-24/2023-24 ADS&AI Assessment Rubric Y2A.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\AAI-DM\docs\Year2\BlockA\MS Teams Assignment Template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\AAI-DM\docs\Year2\BlockA\MS Teams Assignment Template\2023-24\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAC758EA-8D9C-4FA6-B846-07D0B2859830}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B909F53E-FC03-439B-AD96-C73A8F96E890}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1068" yWindow="-108" windowWidth="22080" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -689,9 +689,6 @@
     <t>2023-24A FGA2.P1-ADSAI</t>
   </si>
   <si>
-    <t>5pm Friday 30th October</t>
-  </si>
-  <si>
     <t xml:space="preserve">Clear comments per submission. All docementation required is present. Submissions are thouroughly checked before submitting. And meeting all criteria in insufficient. </t>
   </si>
   <si>
@@ -787,6 +784,9 @@
   </si>
   <si>
     <t>Individual contribution to quantitative and qualitative study design and data collection is clearly documented.</t>
+  </si>
+  <si>
+    <t>5pm Friday 3th November</t>
   </si>
 </sst>
 </file>
@@ -1554,21 +1554,107 @@
     <xf numFmtId="0" fontId="26" fillId="48" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="27" fillId="49" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="47" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="47" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="47" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="47" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="47" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="39" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="22" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="40" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="41" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="42" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1581,104 +1667,21 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="41" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="22" fillId="41" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="45" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="40" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="41" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="41" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="22" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="47" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="39" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="47" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="47" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="47" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="47" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1692,9 +1695,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -2026,10 +2026,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
@@ -2235,8 +2231,8 @@
   <dimension ref="A1:W54"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="10" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I20" sqref="I20"/>
+      <pane ySplit="10" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
@@ -2278,11 +2274,11 @@
     <row r="2" spans="1:16" ht="23.4">
       <c r="A2" s="17"/>
       <c r="B2" s="18"/>
-      <c r="C2" s="102" t="s">
+      <c r="C2" s="101" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="103"/>
-      <c r="E2" s="103"/>
+      <c r="D2" s="102"/>
+      <c r="E2" s="102"/>
       <c r="F2" s="18"/>
       <c r="G2" s="18"/>
       <c r="H2" s="18"/>
@@ -2298,8 +2294,8 @@
     <row r="3" spans="1:16" s="23" customFormat="1" ht="14.4" customHeight="1">
       <c r="A3" s="19"/>
       <c r="B3" s="20"/>
-      <c r="C3" s="121"/>
-      <c r="D3" s="122"/>
+      <c r="C3" s="114"/>
+      <c r="D3" s="115"/>
       <c r="E3" s="38" t="s">
         <v>1</v>
       </c>
@@ -2309,40 +2305,40 @@
       <c r="G3" s="21"/>
       <c r="H3" s="22"/>
       <c r="I3" s="22"/>
-      <c r="J3" s="105" t="s">
+      <c r="J3" s="116" t="s">
         <v>3</v>
       </c>
-      <c r="K3" s="123"/>
-      <c r="L3" s="124" t="s">
+      <c r="K3" s="117"/>
+      <c r="L3" s="118" t="s">
         <v>4</v>
       </c>
-      <c r="M3" s="103"/>
-      <c r="N3" s="103"/>
+      <c r="M3" s="102"/>
+      <c r="N3" s="102"/>
       <c r="O3" s="20"/>
       <c r="P3" s="19"/>
     </row>
     <row r="4" spans="1:16" ht="12.9" customHeight="1">
       <c r="A4" s="17"/>
       <c r="B4" s="24"/>
-      <c r="C4" s="125" t="s">
+      <c r="C4" s="119" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="103"/>
+      <c r="D4" s="102"/>
       <c r="E4" s="15"/>
-      <c r="F4" s="126"/>
-      <c r="G4" s="127"/>
-      <c r="H4" s="127"/>
-      <c r="I4" s="127"/>
-      <c r="J4" s="128"/>
-      <c r="K4" s="129"/>
-      <c r="L4" s="130" t="s">
+      <c r="F4" s="120"/>
+      <c r="G4" s="121"/>
+      <c r="H4" s="121"/>
+      <c r="I4" s="121"/>
+      <c r="J4" s="122"/>
+      <c r="K4" s="123"/>
+      <c r="L4" s="124" t="s">
         <v>6</v>
       </c>
-      <c r="M4" s="131">
+      <c r="M4" s="125">
         <f>IF(ROUND((N24/10),1)&lt;&gt;ROUND((N24/10),0),ROUND((N2/10),1),ROUND((N24/10),0))</f>
         <v>0</v>
       </c>
-      <c r="N4" s="132" t="str">
+      <c r="N4" s="126" t="str">
         <f>IF(M4&gt;=5.5,"PASS",IF(M4&gt;0,"FAIL","M/O"))</f>
         <v>M/O</v>
       </c>
@@ -2352,86 +2348,86 @@
     <row r="5" spans="1:16" ht="12.9" customHeight="1">
       <c r="A5" s="17"/>
       <c r="B5" s="24"/>
-      <c r="C5" s="125" t="s">
+      <c r="C5" s="119" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="123"/>
+      <c r="D5" s="117"/>
       <c r="E5" s="15"/>
-      <c r="F5" s="127"/>
-      <c r="G5" s="127"/>
-      <c r="H5" s="127"/>
-      <c r="I5" s="127"/>
-      <c r="J5" s="129"/>
-      <c r="K5" s="129"/>
-      <c r="L5" s="123"/>
-      <c r="M5" s="123"/>
-      <c r="N5" s="123"/>
+      <c r="F5" s="121"/>
+      <c r="G5" s="121"/>
+      <c r="H5" s="121"/>
+      <c r="I5" s="121"/>
+      <c r="J5" s="123"/>
+      <c r="K5" s="123"/>
+      <c r="L5" s="117"/>
+      <c r="M5" s="117"/>
+      <c r="N5" s="117"/>
       <c r="O5" s="18"/>
       <c r="P5" s="17"/>
     </row>
     <row r="6" spans="1:16" ht="13.8">
       <c r="A6" s="17"/>
       <c r="B6" s="24"/>
-      <c r="C6" s="125" t="s">
+      <c r="C6" s="119" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="133"/>
+      <c r="D6" s="127"/>
       <c r="E6" s="96" t="s">
         <v>188</v>
       </c>
-      <c r="F6" s="127"/>
-      <c r="G6" s="127"/>
-      <c r="H6" s="127"/>
-      <c r="I6" s="127"/>
-      <c r="J6" s="129"/>
-      <c r="K6" s="129"/>
-      <c r="L6" s="123"/>
-      <c r="M6" s="123"/>
-      <c r="N6" s="123"/>
+      <c r="F6" s="121"/>
+      <c r="G6" s="121"/>
+      <c r="H6" s="121"/>
+      <c r="I6" s="121"/>
+      <c r="J6" s="123"/>
+      <c r="K6" s="123"/>
+      <c r="L6" s="117"/>
+      <c r="M6" s="117"/>
+      <c r="N6" s="117"/>
       <c r="O6" s="18"/>
       <c r="P6" s="17"/>
     </row>
     <row r="7" spans="1:16" ht="13.8">
       <c r="A7" s="17"/>
       <c r="B7" s="24"/>
-      <c r="C7" s="125" t="s">
+      <c r="C7" s="119" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="123"/>
+      <c r="D7" s="117"/>
       <c r="E7" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="127"/>
-      <c r="G7" s="127"/>
-      <c r="H7" s="127"/>
-      <c r="I7" s="127"/>
-      <c r="J7" s="129"/>
-      <c r="K7" s="129"/>
-      <c r="L7" s="123"/>
-      <c r="M7" s="123"/>
-      <c r="N7" s="123"/>
+      <c r="F7" s="121"/>
+      <c r="G7" s="121"/>
+      <c r="H7" s="121"/>
+      <c r="I7" s="121"/>
+      <c r="J7" s="123"/>
+      <c r="K7" s="123"/>
+      <c r="L7" s="117"/>
+      <c r="M7" s="117"/>
+      <c r="N7" s="117"/>
       <c r="O7" s="18"/>
       <c r="P7" s="17"/>
     </row>
     <row r="8" spans="1:16" ht="28.35" customHeight="1">
       <c r="A8" s="17"/>
       <c r="B8" s="24"/>
-      <c r="C8" s="134" t="s">
+      <c r="C8" s="128" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="135"/>
+      <c r="D8" s="129"/>
       <c r="E8" s="40" t="s">
-        <v>189</v>
-      </c>
-      <c r="F8" s="127"/>
-      <c r="G8" s="127"/>
-      <c r="H8" s="127"/>
-      <c r="I8" s="127"/>
-      <c r="J8" s="129"/>
-      <c r="K8" s="129"/>
-      <c r="L8" s="123"/>
-      <c r="M8" s="123"/>
-      <c r="N8" s="123"/>
+        <v>207</v>
+      </c>
+      <c r="F8" s="121"/>
+      <c r="G8" s="121"/>
+      <c r="H8" s="121"/>
+      <c r="I8" s="121"/>
+      <c r="J8" s="123"/>
+      <c r="K8" s="123"/>
+      <c r="L8" s="117"/>
+      <c r="M8" s="117"/>
+      <c r="N8" s="117"/>
       <c r="O8" s="18"/>
       <c r="P8" s="17"/>
     </row>
@@ -2474,11 +2470,11 @@
     <row r="11" spans="1:16" ht="23.4">
       <c r="A11" s="17"/>
       <c r="B11" s="18"/>
-      <c r="C11" s="102" t="s">
+      <c r="C11" s="101" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="103"/>
-      <c r="E11" s="103"/>
+      <c r="D11" s="102"/>
+      <c r="E11" s="102"/>
       <c r="F11" s="18"/>
       <c r="G11" s="18"/>
       <c r="H11" s="18"/>
@@ -2534,19 +2530,19 @@
     <row r="13" spans="1:16" ht="48.6" customHeight="1">
       <c r="A13" s="17"/>
       <c r="B13" s="27"/>
-      <c r="C13" s="136">
+      <c r="C13" s="103">
         <v>9</v>
       </c>
-      <c r="D13" s="143" t="s">
-        <v>196</v>
-      </c>
-      <c r="E13" s="143"/>
-      <c r="F13" s="143"/>
-      <c r="G13" s="143"/>
-      <c r="H13" s="143"/>
-      <c r="I13" s="143"/>
-      <c r="J13" s="143"/>
-      <c r="K13" s="143"/>
+      <c r="D13" s="104" t="s">
+        <v>195</v>
+      </c>
+      <c r="E13" s="104"/>
+      <c r="F13" s="104"/>
+      <c r="G13" s="104"/>
+      <c r="H13" s="104"/>
+      <c r="I13" s="104"/>
+      <c r="J13" s="104"/>
+      <c r="K13" s="104"/>
       <c r="L13" s="82"/>
       <c r="M13" s="82"/>
       <c r="N13" s="82"/>
@@ -2556,22 +2552,22 @@
     <row r="14" spans="1:16" ht="118.65" customHeight="1">
       <c r="A14" s="17"/>
       <c r="B14" s="18"/>
-      <c r="C14" s="136"/>
-      <c r="D14" s="144" t="s">
+      <c r="C14" s="103"/>
+      <c r="D14" s="105" t="s">
         <v>23</v>
       </c>
-      <c r="E14" s="144"/>
+      <c r="E14" s="105"/>
       <c r="F14" s="81" t="s">
         <v>24</v>
       </c>
       <c r="G14" s="51" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H14" s="52" t="s">
         <v>25</v>
       </c>
       <c r="I14" s="53" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="J14" s="54" t="s">
         <v>185</v>
@@ -2596,16 +2592,16 @@
       <c r="A15" s="17"/>
       <c r="B15" s="27"/>
       <c r="C15" s="95"/>
-      <c r="D15" s="145" t="s">
-        <v>195</v>
-      </c>
-      <c r="E15" s="139"/>
-      <c r="F15" s="139"/>
-      <c r="G15" s="139"/>
-      <c r="H15" s="139"/>
-      <c r="I15" s="139"/>
-      <c r="J15" s="139"/>
-      <c r="K15" s="139"/>
+      <c r="D15" s="106" t="s">
+        <v>194</v>
+      </c>
+      <c r="E15" s="107"/>
+      <c r="F15" s="107"/>
+      <c r="G15" s="107"/>
+      <c r="H15" s="107"/>
+      <c r="I15" s="107"/>
+      <c r="J15" s="107"/>
+      <c r="K15" s="107"/>
       <c r="L15" s="83"/>
       <c r="M15" s="83"/>
       <c r="N15" s="83"/>
@@ -2618,10 +2614,10 @@
       <c r="C16" s="95" t="s">
         <v>26</v>
       </c>
-      <c r="D16" s="119" t="s">
+      <c r="D16" s="99" t="s">
         <v>27</v>
       </c>
-      <c r="E16" s="140"/>
+      <c r="E16" s="100"/>
       <c r="F16" s="81" t="s">
         <v>24</v>
       </c>
@@ -2656,19 +2652,19 @@
     <row r="17" spans="1:23" ht="48" customHeight="1">
       <c r="A17" s="17"/>
       <c r="B17" s="27"/>
-      <c r="C17" s="138" t="s">
+      <c r="C17" s="110" t="s">
         <v>32</v>
       </c>
-      <c r="D17" s="139" t="s">
-        <v>197</v>
-      </c>
-      <c r="E17" s="139"/>
-      <c r="F17" s="139"/>
-      <c r="G17" s="139"/>
-      <c r="H17" s="139"/>
-      <c r="I17" s="139"/>
-      <c r="J17" s="139"/>
-      <c r="K17" s="139"/>
+      <c r="D17" s="107" t="s">
+        <v>196</v>
+      </c>
+      <c r="E17" s="107"/>
+      <c r="F17" s="107"/>
+      <c r="G17" s="107"/>
+      <c r="H17" s="107"/>
+      <c r="I17" s="107"/>
+      <c r="J17" s="107"/>
+      <c r="K17" s="107"/>
       <c r="L17" s="83"/>
       <c r="M17" s="83"/>
       <c r="N17" s="83"/>
@@ -2685,28 +2681,28 @@
     <row r="18" spans="1:23" ht="111.9" customHeight="1">
       <c r="A18" s="17"/>
       <c r="B18" s="18"/>
-      <c r="C18" s="138"/>
-      <c r="D18" s="119" t="s">
+      <c r="C18" s="110"/>
+      <c r="D18" s="99" t="s">
         <v>186</v>
       </c>
-      <c r="E18" s="140"/>
+      <c r="E18" s="100"/>
       <c r="F18" s="81" t="s">
         <v>24</v>
       </c>
       <c r="G18" s="51" t="s">
+        <v>197</v>
+      </c>
+      <c r="H18" s="52" t="s">
+        <v>191</v>
+      </c>
+      <c r="I18" s="53" t="s">
+        <v>192</v>
+      </c>
+      <c r="J18" s="54" t="s">
+        <v>193</v>
+      </c>
+      <c r="K18" s="55" t="s">
         <v>198</v>
-      </c>
-      <c r="H18" s="52" t="s">
-        <v>192</v>
-      </c>
-      <c r="I18" s="53" t="s">
-        <v>193</v>
-      </c>
-      <c r="J18" s="54" t="s">
-        <v>194</v>
-      </c>
-      <c r="K18" s="55" t="s">
-        <v>199</v>
       </c>
       <c r="L18" s="42">
         <v>10</v>
@@ -2731,19 +2727,19 @@
     <row r="19" spans="1:23" ht="42.9" customHeight="1">
       <c r="A19" s="17"/>
       <c r="B19" s="27"/>
-      <c r="C19" s="136">
+      <c r="C19" s="103">
         <v>3</v>
       </c>
-      <c r="D19" s="151" t="s">
+      <c r="D19" s="111" t="s">
         <v>33</v>
       </c>
-      <c r="E19" s="141"/>
-      <c r="F19" s="141"/>
-      <c r="G19" s="141"/>
-      <c r="H19" s="141"/>
-      <c r="I19" s="141"/>
-      <c r="J19" s="141"/>
-      <c r="K19" s="141"/>
+      <c r="E19" s="112"/>
+      <c r="F19" s="112"/>
+      <c r="G19" s="112"/>
+      <c r="H19" s="112"/>
+      <c r="I19" s="112"/>
+      <c r="J19" s="112"/>
+      <c r="K19" s="112"/>
       <c r="L19" s="46"/>
       <c r="M19" s="46"/>
       <c r="N19" s="46"/>
@@ -2760,25 +2756,25 @@
     <row r="20" spans="1:23" s="57" customFormat="1" ht="111.9" customHeight="1">
       <c r="A20" s="49"/>
       <c r="B20" s="50"/>
-      <c r="C20" s="103"/>
-      <c r="D20" s="142" t="s">
+      <c r="C20" s="102"/>
+      <c r="D20" s="113" t="s">
         <v>34</v>
       </c>
-      <c r="E20" s="142"/>
+      <c r="E20" s="113"/>
       <c r="F20" s="81" t="s">
         <v>24</v>
       </c>
       <c r="G20" s="60" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="H20" s="61" t="s">
+        <v>199</v>
+      </c>
+      <c r="I20" s="62" t="s">
         <v>200</v>
       </c>
-      <c r="I20" s="62" t="s">
+      <c r="J20" s="63" t="s">
         <v>201</v>
-      </c>
-      <c r="J20" s="63" t="s">
-        <v>202</v>
       </c>
       <c r="K20" s="64" t="s">
         <v>177</v>
@@ -2806,17 +2802,17 @@
     <row r="21" spans="1:23" ht="53.1" customHeight="1">
       <c r="A21" s="17"/>
       <c r="B21" s="18"/>
-      <c r="C21" s="136" t="s">
+      <c r="C21" s="103" t="s">
         <v>35</v>
       </c>
-      <c r="D21" s="137" t="s">
+      <c r="D21" s="108" t="s">
         <v>36</v>
       </c>
-      <c r="E21" s="118"/>
-      <c r="F21" s="118"/>
-      <c r="G21" s="118"/>
-      <c r="H21" s="118"/>
-      <c r="I21" s="118"/>
+      <c r="E21" s="109"/>
+      <c r="F21" s="109"/>
+      <c r="G21" s="109"/>
+      <c r="H21" s="109"/>
+      <c r="I21" s="109"/>
       <c r="J21" s="86"/>
       <c r="K21" s="86"/>
       <c r="L21" s="83"/>
@@ -2835,16 +2831,16 @@
     <row r="22" spans="1:23" ht="138.75" customHeight="1">
       <c r="A22" s="17"/>
       <c r="B22" s="18"/>
-      <c r="C22" s="103"/>
-      <c r="D22" s="119" t="s">
+      <c r="C22" s="102"/>
+      <c r="D22" s="99" t="s">
         <v>37</v>
       </c>
-      <c r="E22" s="119"/>
+      <c r="E22" s="99"/>
       <c r="F22" s="81" t="s">
         <v>24</v>
       </c>
       <c r="G22" s="58" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="H22" s="41" t="s">
         <v>38</v>
@@ -2882,14 +2878,14 @@
       <c r="A23" s="17"/>
       <c r="B23" s="18"/>
       <c r="C23" s="59"/>
-      <c r="D23" s="118" t="s">
+      <c r="D23" s="109" t="s">
         <v>41</v>
       </c>
-      <c r="E23" s="118"/>
-      <c r="F23" s="118"/>
-      <c r="G23" s="118"/>
-      <c r="H23" s="118"/>
-      <c r="I23" s="118"/>
+      <c r="E23" s="109"/>
+      <c r="F23" s="109"/>
+      <c r="G23" s="109"/>
+      <c r="H23" s="109"/>
+      <c r="I23" s="109"/>
       <c r="J23" s="86"/>
       <c r="K23" s="86"/>
       <c r="L23" s="83"/>
@@ -2911,18 +2907,18 @@
       <c r="C24" s="59" t="s">
         <v>42</v>
       </c>
-      <c r="D24" s="119" t="s">
+      <c r="D24" s="99" t="s">
         <v>43</v>
       </c>
-      <c r="E24" s="119"/>
+      <c r="E24" s="99"/>
       <c r="F24" s="81" t="s">
         <v>24</v>
       </c>
       <c r="G24" s="58" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="H24" s="41" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="I24" s="47" t="s">
         <v>44</v>
@@ -2957,14 +2953,14 @@
       <c r="A25" s="17"/>
       <c r="B25" s="18"/>
       <c r="C25" s="59"/>
-      <c r="D25" s="118" t="s">
+      <c r="D25" s="109" t="s">
         <v>183</v>
       </c>
-      <c r="E25" s="118"/>
-      <c r="F25" s="118"/>
-      <c r="G25" s="118"/>
-      <c r="H25" s="118"/>
-      <c r="I25" s="118"/>
+      <c r="E25" s="109"/>
+      <c r="F25" s="109"/>
+      <c r="G25" s="109"/>
+      <c r="H25" s="109"/>
+      <c r="I25" s="109"/>
       <c r="J25" s="86"/>
       <c r="K25" s="86"/>
       <c r="L25" s="83"/>
@@ -2986,15 +2982,15 @@
       <c r="C26" s="59" t="s">
         <v>42</v>
       </c>
-      <c r="D26" s="119" t="s">
+      <c r="D26" s="99" t="s">
         <v>184</v>
       </c>
-      <c r="E26" s="119"/>
+      <c r="E26" s="99"/>
       <c r="F26" s="81" t="s">
         <v>24</v>
       </c>
       <c r="G26" s="58" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="H26" s="41" t="s">
         <v>47</v>
@@ -3084,11 +3080,11 @@
     <row r="29" spans="1:23" s="59" customFormat="1" ht="23.4">
       <c r="A29" s="17"/>
       <c r="B29" s="29"/>
-      <c r="C29" s="102" t="s">
+      <c r="C29" s="101" t="s">
         <v>51</v>
       </c>
-      <c r="D29" s="103"/>
-      <c r="E29" s="103"/>
+      <c r="D29" s="102"/>
+      <c r="E29" s="102"/>
       <c r="F29" s="29"/>
       <c r="G29" s="29"/>
       <c r="H29" s="29"/>
@@ -3107,20 +3103,20 @@
       <c r="C30" s="89" t="s">
         <v>52</v>
       </c>
-      <c r="D30" s="105" t="s">
+      <c r="D30" s="116" t="s">
         <v>53</v>
       </c>
-      <c r="E30" s="103"/>
+      <c r="E30" s="102"/>
       <c r="F30" s="89" t="s">
         <v>54</v>
       </c>
-      <c r="G30" s="105" t="s">
+      <c r="G30" s="116" t="s">
         <v>2</v>
       </c>
-      <c r="H30" s="103"/>
-      <c r="I30" s="103"/>
-      <c r="J30" s="103"/>
-      <c r="K30" s="103"/>
+      <c r="H30" s="102"/>
+      <c r="I30" s="102"/>
+      <c r="J30" s="102"/>
+      <c r="K30" s="102"/>
       <c r="L30" s="65"/>
       <c r="M30" s="89"/>
       <c r="N30" s="92" t="s">
@@ -3135,22 +3131,22 @@
       <c r="C31" s="66">
         <v>9</v>
       </c>
-      <c r="D31" s="115" t="s">
+      <c r="D31" s="133" t="s">
         <v>56</v>
       </c>
-      <c r="E31" s="116"/>
+      <c r="E31" s="131"/>
       <c r="F31" s="91" t="s">
         <v>57</v>
       </c>
-      <c r="G31" s="117" t="s">
+      <c r="G31" s="132" t="s">
         <v>58</v>
       </c>
-      <c r="H31" s="117"/>
-      <c r="I31" s="117"/>
-      <c r="J31" s="117"/>
-      <c r="K31" s="117"/>
-      <c r="L31" s="117"/>
-      <c r="M31" s="117"/>
+      <c r="H31" s="132"/>
+      <c r="I31" s="132"/>
+      <c r="J31" s="132"/>
+      <c r="K31" s="132"/>
+      <c r="L31" s="132"/>
+      <c r="M31" s="132"/>
       <c r="N31" s="67">
         <v>3</v>
       </c>
@@ -3163,22 +3159,22 @@
       <c r="C32" s="68">
         <v>10</v>
       </c>
-      <c r="D32" s="120" t="s">
+      <c r="D32" s="130" t="s">
         <v>56</v>
       </c>
-      <c r="E32" s="116"/>
+      <c r="E32" s="131"/>
       <c r="F32" s="91" t="s">
         <v>59</v>
       </c>
-      <c r="G32" s="117" t="s">
+      <c r="G32" s="132" t="s">
         <v>60</v>
       </c>
-      <c r="H32" s="117"/>
-      <c r="I32" s="117"/>
-      <c r="J32" s="117"/>
-      <c r="K32" s="117"/>
-      <c r="L32" s="117"/>
-      <c r="M32" s="117"/>
+      <c r="H32" s="132"/>
+      <c r="I32" s="132"/>
+      <c r="J32" s="132"/>
+      <c r="K32" s="132"/>
+      <c r="L32" s="132"/>
+      <c r="M32" s="132"/>
       <c r="N32" s="69">
         <v>3</v>
       </c>
@@ -3191,22 +3187,22 @@
       <c r="C33" s="66">
         <v>11</v>
       </c>
-      <c r="D33" s="115" t="s">
+      <c r="D33" s="133" t="s">
         <v>56</v>
       </c>
-      <c r="E33" s="116"/>
+      <c r="E33" s="131"/>
       <c r="F33" s="91" t="s">
         <v>61</v>
       </c>
-      <c r="G33" s="117" t="s">
+      <c r="G33" s="132" t="s">
         <v>62</v>
       </c>
-      <c r="H33" s="117"/>
-      <c r="I33" s="117"/>
-      <c r="J33" s="117"/>
-      <c r="K33" s="117"/>
-      <c r="L33" s="117"/>
-      <c r="M33" s="117"/>
+      <c r="H33" s="132"/>
+      <c r="I33" s="132"/>
+      <c r="J33" s="132"/>
+      <c r="K33" s="132"/>
+      <c r="L33" s="132"/>
+      <c r="M33" s="132"/>
       <c r="N33" s="67">
         <v>3</v>
       </c>
@@ -3219,22 +3215,22 @@
       <c r="C34" s="70">
         <v>1</v>
       </c>
-      <c r="D34" s="113" t="s">
+      <c r="D34" s="134" t="s">
         <v>63</v>
       </c>
-      <c r="E34" s="113"/>
+      <c r="E34" s="134"/>
       <c r="F34" s="90" t="s">
         <v>64</v>
       </c>
-      <c r="G34" s="111" t="s">
+      <c r="G34" s="135" t="s">
         <v>182</v>
       </c>
-      <c r="H34" s="111"/>
-      <c r="I34" s="111"/>
-      <c r="J34" s="111"/>
-      <c r="K34" s="111"/>
-      <c r="L34" s="111"/>
-      <c r="M34" s="111"/>
+      <c r="H34" s="135"/>
+      <c r="I34" s="135"/>
+      <c r="J34" s="135"/>
+      <c r="K34" s="135"/>
+      <c r="L34" s="135"/>
+      <c r="M34" s="135"/>
       <c r="N34" s="71">
         <v>3</v>
       </c>
@@ -3247,22 +3243,22 @@
       <c r="C35" s="72">
         <v>2</v>
       </c>
-      <c r="D35" s="106" t="s">
+      <c r="D35" s="136" t="s">
         <v>63</v>
       </c>
-      <c r="E35" s="107"/>
+      <c r="E35" s="137"/>
       <c r="F35" s="87" t="s">
         <v>65</v>
       </c>
-      <c r="G35" s="108" t="s">
+      <c r="G35" s="138" t="s">
         <v>66</v>
       </c>
-      <c r="H35" s="108"/>
-      <c r="I35" s="108"/>
-      <c r="J35" s="108"/>
-      <c r="K35" s="108"/>
-      <c r="L35" s="108"/>
-      <c r="M35" s="108"/>
+      <c r="H35" s="138"/>
+      <c r="I35" s="138"/>
+      <c r="J35" s="138"/>
+      <c r="K35" s="138"/>
+      <c r="L35" s="138"/>
+      <c r="M35" s="138"/>
       <c r="N35" s="73">
         <v>3</v>
       </c>
@@ -3275,22 +3271,22 @@
       <c r="C36" s="74">
         <v>3</v>
       </c>
-      <c r="D36" s="109" t="s">
+      <c r="D36" s="139" t="s">
         <v>67</v>
       </c>
-      <c r="E36" s="110"/>
+      <c r="E36" s="140"/>
       <c r="F36" s="90" t="s">
         <v>68</v>
       </c>
-      <c r="G36" s="111" t="s">
+      <c r="G36" s="135" t="s">
         <v>69</v>
       </c>
-      <c r="H36" s="111"/>
-      <c r="I36" s="111"/>
-      <c r="J36" s="111"/>
-      <c r="K36" s="111"/>
-      <c r="L36" s="111"/>
-      <c r="M36" s="111"/>
+      <c r="H36" s="135"/>
+      <c r="I36" s="135"/>
+      <c r="J36" s="135"/>
+      <c r="K36" s="135"/>
+      <c r="L36" s="135"/>
+      <c r="M36" s="135"/>
       <c r="N36" s="75">
         <v>3</v>
       </c>
@@ -3303,22 +3299,22 @@
       <c r="C37" s="76">
         <v>4</v>
       </c>
-      <c r="D37" s="112" t="s">
+      <c r="D37" s="141" t="s">
         <v>70</v>
       </c>
-      <c r="E37" s="107"/>
+      <c r="E37" s="137"/>
       <c r="F37" s="87" t="s">
         <v>71</v>
       </c>
-      <c r="G37" s="108" t="s">
+      <c r="G37" s="138" t="s">
         <v>179</v>
       </c>
-      <c r="H37" s="108"/>
-      <c r="I37" s="108"/>
-      <c r="J37" s="108"/>
-      <c r="K37" s="108"/>
-      <c r="L37" s="108"/>
-      <c r="M37" s="108"/>
+      <c r="H37" s="138"/>
+      <c r="I37" s="138"/>
+      <c r="J37" s="138"/>
+      <c r="K37" s="138"/>
+      <c r="L37" s="138"/>
+      <c r="M37" s="138"/>
       <c r="N37" s="77">
         <v>3</v>
       </c>
@@ -3331,22 +3327,22 @@
       <c r="C38" s="70">
         <v>5</v>
       </c>
-      <c r="D38" s="113" t="s">
+      <c r="D38" s="134" t="s">
         <v>72</v>
       </c>
-      <c r="E38" s="114"/>
+      <c r="E38" s="142"/>
       <c r="F38" s="90" t="s">
         <v>72</v>
       </c>
-      <c r="G38" s="111" t="s">
+      <c r="G38" s="135" t="s">
         <v>180</v>
       </c>
-      <c r="H38" s="111"/>
-      <c r="I38" s="111"/>
-      <c r="J38" s="111"/>
-      <c r="K38" s="111"/>
-      <c r="L38" s="111"/>
-      <c r="M38" s="111"/>
+      <c r="H38" s="135"/>
+      <c r="I38" s="135"/>
+      <c r="J38" s="135"/>
+      <c r="K38" s="135"/>
+      <c r="L38" s="135"/>
+      <c r="M38" s="135"/>
       <c r="N38" s="71">
         <v>3</v>
       </c>
@@ -3359,22 +3355,22 @@
       <c r="C39" s="72">
         <v>6</v>
       </c>
-      <c r="D39" s="106" t="s">
+      <c r="D39" s="136" t="s">
         <v>72</v>
       </c>
-      <c r="E39" s="107"/>
+      <c r="E39" s="137"/>
       <c r="F39" s="87" t="s">
         <v>73</v>
       </c>
-      <c r="G39" s="108" t="s">
+      <c r="G39" s="138" t="s">
         <v>181</v>
       </c>
-      <c r="H39" s="108"/>
-      <c r="I39" s="108"/>
-      <c r="J39" s="108"/>
-      <c r="K39" s="108"/>
-      <c r="L39" s="108"/>
-      <c r="M39" s="108"/>
+      <c r="H39" s="138"/>
+      <c r="I39" s="138"/>
+      <c r="J39" s="138"/>
+      <c r="K39" s="138"/>
+      <c r="L39" s="138"/>
+      <c r="M39" s="138"/>
       <c r="N39" s="73">
         <v>3</v>
       </c>
@@ -3387,22 +3383,22 @@
       <c r="C40" s="74">
         <v>7</v>
       </c>
-      <c r="D40" s="109" t="s">
+      <c r="D40" s="139" t="s">
         <v>74</v>
       </c>
-      <c r="E40" s="110"/>
+      <c r="E40" s="140"/>
       <c r="F40" s="90" t="s">
         <v>75</v>
       </c>
-      <c r="G40" s="111" t="s">
+      <c r="G40" s="135" t="s">
         <v>76</v>
       </c>
-      <c r="H40" s="111"/>
-      <c r="I40" s="111"/>
-      <c r="J40" s="111"/>
-      <c r="K40" s="111"/>
-      <c r="L40" s="111"/>
-      <c r="M40" s="111"/>
+      <c r="H40" s="135"/>
+      <c r="I40" s="135"/>
+      <c r="J40" s="135"/>
+      <c r="K40" s="135"/>
+      <c r="L40" s="135"/>
+      <c r="M40" s="135"/>
       <c r="N40" s="75">
         <v>3</v>
       </c>
@@ -3415,22 +3411,22 @@
       <c r="C41" s="76">
         <v>8</v>
       </c>
-      <c r="D41" s="112" t="s">
+      <c r="D41" s="141" t="s">
         <v>74</v>
       </c>
-      <c r="E41" s="107"/>
+      <c r="E41" s="137"/>
       <c r="F41" s="87" t="s">
         <v>77</v>
       </c>
-      <c r="G41" s="108" t="s">
+      <c r="G41" s="138" t="s">
         <v>78</v>
       </c>
-      <c r="H41" s="108"/>
-      <c r="I41" s="108"/>
-      <c r="J41" s="108"/>
-      <c r="K41" s="108"/>
-      <c r="L41" s="108"/>
-      <c r="M41" s="108"/>
+      <c r="H41" s="138"/>
+      <c r="I41" s="138"/>
+      <c r="J41" s="138"/>
+      <c r="K41" s="138"/>
+      <c r="L41" s="138"/>
+      <c r="M41" s="138"/>
       <c r="N41" s="77">
         <v>3</v>
       </c>
@@ -3476,11 +3472,11 @@
     <row r="44" spans="1:16" s="59" customFormat="1" ht="23.4">
       <c r="A44" s="17"/>
       <c r="B44" s="32"/>
-      <c r="C44" s="102" t="s">
+      <c r="C44" s="101" t="s">
         <v>79</v>
       </c>
-      <c r="D44" s="103"/>
-      <c r="E44" s="103"/>
+      <c r="D44" s="102"/>
+      <c r="E44" s="102"/>
       <c r="F44" s="27"/>
       <c r="G44" s="18"/>
       <c r="H44" s="18"/>
@@ -3503,19 +3499,19 @@
         <v>80</v>
       </c>
       <c r="E45" s="88"/>
-      <c r="F45" s="104" t="s">
+      <c r="F45" s="143" t="s">
         <v>81</v>
       </c>
-      <c r="G45" s="103"/>
-      <c r="H45" s="103"/>
-      <c r="I45" s="103"/>
-      <c r="J45" s="105" t="s">
+      <c r="G45" s="102"/>
+      <c r="H45" s="102"/>
+      <c r="I45" s="102"/>
+      <c r="J45" s="116" t="s">
         <v>82</v>
       </c>
-      <c r="K45" s="103"/>
-      <c r="L45" s="103"/>
-      <c r="M45" s="103"/>
-      <c r="N45" s="103"/>
+      <c r="K45" s="102"/>
+      <c r="L45" s="102"/>
+      <c r="M45" s="102"/>
+      <c r="N45" s="102"/>
       <c r="O45" s="18"/>
       <c r="P45" s="17"/>
     </row>
@@ -3529,19 +3525,19 @@
         <v>83</v>
       </c>
       <c r="E46" s="85"/>
-      <c r="F46" s="99" t="s">
+      <c r="F46" s="146" t="s">
         <v>84</v>
       </c>
-      <c r="G46" s="100"/>
-      <c r="H46" s="100"/>
-      <c r="I46" s="100"/>
-      <c r="J46" s="99" t="s">
+      <c r="G46" s="145"/>
+      <c r="H46" s="145"/>
+      <c r="I46" s="145"/>
+      <c r="J46" s="146" t="s">
         <v>85</v>
       </c>
-      <c r="K46" s="100"/>
-      <c r="L46" s="100"/>
-      <c r="M46" s="100"/>
-      <c r="N46" s="100"/>
+      <c r="K46" s="145"/>
+      <c r="L46" s="145"/>
+      <c r="M46" s="145"/>
+      <c r="N46" s="145"/>
       <c r="O46" s="18"/>
       <c r="P46" s="17"/>
     </row>
@@ -3555,19 +3551,19 @@
         <v>86</v>
       </c>
       <c r="E47" s="84"/>
-      <c r="F47" s="101" t="s">
+      <c r="F47" s="144" t="s">
         <v>87</v>
       </c>
-      <c r="G47" s="100"/>
-      <c r="H47" s="100"/>
-      <c r="I47" s="100"/>
-      <c r="J47" s="101" t="s">
+      <c r="G47" s="145"/>
+      <c r="H47" s="145"/>
+      <c r="I47" s="145"/>
+      <c r="J47" s="144" t="s">
         <v>88</v>
       </c>
-      <c r="K47" s="100"/>
-      <c r="L47" s="100"/>
-      <c r="M47" s="100"/>
-      <c r="N47" s="100"/>
+      <c r="K47" s="145"/>
+      <c r="L47" s="145"/>
+      <c r="M47" s="145"/>
+      <c r="N47" s="145"/>
       <c r="O47" s="18"/>
       <c r="P47" s="17"/>
     </row>
@@ -3581,19 +3577,19 @@
         <v>89</v>
       </c>
       <c r="E48" s="85"/>
-      <c r="F48" s="99" t="s">
+      <c r="F48" s="146" t="s">
         <v>90</v>
       </c>
-      <c r="G48" s="100"/>
-      <c r="H48" s="100"/>
-      <c r="I48" s="100"/>
-      <c r="J48" s="99" t="s">
+      <c r="G48" s="145"/>
+      <c r="H48" s="145"/>
+      <c r="I48" s="145"/>
+      <c r="J48" s="146" t="s">
         <v>91</v>
       </c>
-      <c r="K48" s="100"/>
-      <c r="L48" s="100"/>
-      <c r="M48" s="100"/>
-      <c r="N48" s="100"/>
+      <c r="K48" s="145"/>
+      <c r="L48" s="145"/>
+      <c r="M48" s="145"/>
+      <c r="N48" s="145"/>
       <c r="O48" s="18"/>
       <c r="P48" s="17"/>
     </row>
@@ -3607,19 +3603,19 @@
         <v>92</v>
       </c>
       <c r="E49" s="84"/>
-      <c r="F49" s="101" t="s">
+      <c r="F49" s="144" t="s">
         <v>93</v>
       </c>
-      <c r="G49" s="100"/>
-      <c r="H49" s="100"/>
-      <c r="I49" s="100"/>
-      <c r="J49" s="101" t="s">
+      <c r="G49" s="145"/>
+      <c r="H49" s="145"/>
+      <c r="I49" s="145"/>
+      <c r="J49" s="144" t="s">
         <v>94</v>
       </c>
-      <c r="K49" s="100"/>
-      <c r="L49" s="100"/>
-      <c r="M49" s="100"/>
-      <c r="N49" s="100"/>
+      <c r="K49" s="145"/>
+      <c r="L49" s="145"/>
+      <c r="M49" s="145"/>
+      <c r="N49" s="145"/>
       <c r="O49" s="18"/>
       <c r="P49" s="17"/>
     </row>
@@ -3633,19 +3629,19 @@
         <v>95</v>
       </c>
       <c r="E50" s="85"/>
-      <c r="F50" s="99" t="s">
+      <c r="F50" s="146" t="s">
         <v>96</v>
       </c>
-      <c r="G50" s="100"/>
-      <c r="H50" s="100"/>
-      <c r="I50" s="100"/>
-      <c r="J50" s="99" t="s">
+      <c r="G50" s="145"/>
+      <c r="H50" s="145"/>
+      <c r="I50" s="145"/>
+      <c r="J50" s="146" t="s">
         <v>97</v>
       </c>
-      <c r="K50" s="100"/>
-      <c r="L50" s="100"/>
-      <c r="M50" s="100"/>
-      <c r="N50" s="100"/>
+      <c r="K50" s="145"/>
+      <c r="L50" s="145"/>
+      <c r="M50" s="145"/>
+      <c r="N50" s="145"/>
       <c r="O50" s="18"/>
       <c r="P50" s="17"/>
     </row>
@@ -3730,21 +3726,48 @@
     <protectedRange algorithmName="SHA-512" hashValue="NcQe0VjxFnxU9SziGkmWOoYUYoQ0T62vv+WqFE1sowJD2+jDiq1RKEMS6wObDPCk433k/JG1CTU3j62rwNOzdg==" saltValue="OlYFZTFPx5QDCqKlqXj8fw==" spinCount="100000" sqref="I20" name="Range1_2_1_2"/>
   </protectedRanges>
   <mergeCells count="71">
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="C11:E11"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="D13:K13"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="D15:K15"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="D21:I21"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="D17:K17"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="D19:K19"/>
-    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="F50:I50"/>
+    <mergeCell ref="J50:N50"/>
+    <mergeCell ref="F46:I46"/>
+    <mergeCell ref="J46:N46"/>
+    <mergeCell ref="F47:I47"/>
+    <mergeCell ref="J47:N47"/>
+    <mergeCell ref="F48:I48"/>
+    <mergeCell ref="J48:N48"/>
+    <mergeCell ref="C44:E44"/>
+    <mergeCell ref="F45:I45"/>
+    <mergeCell ref="J45:N45"/>
+    <mergeCell ref="F49:I49"/>
+    <mergeCell ref="J49:N49"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="G39:M39"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="G40:M40"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="G41:M41"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="G36:M36"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="G37:M37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="G38:M38"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="G33:M33"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="G34:M34"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="G35:M35"/>
+    <mergeCell ref="D23:I23"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="D25:I25"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="G32:M32"/>
+    <mergeCell ref="C29:E29"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="G30:K30"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="G31:M31"/>
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="J3:K3"/>
@@ -3759,48 +3782,21 @@
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="C7:D7"/>
     <mergeCell ref="C8:D8"/>
-    <mergeCell ref="D23:I23"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="D25:I25"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="G32:M32"/>
-    <mergeCell ref="C29:E29"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="G30:K30"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="G31:M31"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="G33:M33"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="G34:M34"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="G35:M35"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="G36:M36"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="G37:M37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="G38:M38"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="G39:M39"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="G40:M40"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="G41:M41"/>
-    <mergeCell ref="C44:E44"/>
-    <mergeCell ref="F45:I45"/>
-    <mergeCell ref="J45:N45"/>
-    <mergeCell ref="F49:I49"/>
-    <mergeCell ref="J49:N49"/>
-    <mergeCell ref="F50:I50"/>
-    <mergeCell ref="J50:N50"/>
-    <mergeCell ref="F46:I46"/>
-    <mergeCell ref="J46:N46"/>
-    <mergeCell ref="F47:I47"/>
-    <mergeCell ref="J47:N47"/>
-    <mergeCell ref="F48:I48"/>
-    <mergeCell ref="J48:N48"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="D21:I21"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="D17:K17"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="D19:K19"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="C11:E11"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="D13:K13"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D15:K15"/>
   </mergeCells>
   <conditionalFormatting sqref="N4">
     <cfRule type="containsText" dxfId="32" priority="81" operator="containsText" text="FAIL">
@@ -3960,38 +3956,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
-      <c r="A1" s="123"/>
-      <c r="B1" s="123"/>
-      <c r="C1" s="123"/>
-      <c r="D1" s="123"/>
-      <c r="E1" s="123"/>
-      <c r="F1" s="123"/>
-      <c r="G1" s="123"/>
-      <c r="H1" s="123"/>
+      <c r="A1" s="117"/>
+      <c r="B1" s="117"/>
+      <c r="C1" s="117"/>
+      <c r="D1" s="117"/>
+      <c r="E1" s="117"/>
+      <c r="F1" s="117"/>
+      <c r="G1" s="117"/>
+      <c r="H1" s="117"/>
     </row>
     <row r="2" spans="1:15">
-      <c r="A2" s="123"/>
-      <c r="B2" s="123"/>
-      <c r="C2" s="123"/>
-      <c r="D2" s="123"/>
-      <c r="E2" s="123"/>
-      <c r="F2" s="123"/>
-      <c r="G2" s="123"/>
-      <c r="H2" s="123"/>
+      <c r="A2" s="117"/>
+      <c r="B2" s="117"/>
+      <c r="C2" s="117"/>
+      <c r="D2" s="117"/>
+      <c r="E2" s="117"/>
+      <c r="F2" s="117"/>
+      <c r="G2" s="117"/>
+      <c r="H2" s="117"/>
     </row>
     <row r="3" spans="1:15" ht="15.75" customHeight="1">
-      <c r="A3" s="123"/>
-      <c r="B3" s="123"/>
+      <c r="A3" s="117"/>
+      <c r="B3" s="117"/>
       <c r="C3"/>
-      <c r="D3" s="123"/>
-      <c r="E3" s="123"/>
-      <c r="F3" s="123"/>
-      <c r="G3" s="123"/>
-      <c r="H3" s="123"/>
-      <c r="K3" s="146"/>
-      <c r="L3" s="147"/>
-      <c r="M3" s="147"/>
-      <c r="N3" s="147"/>
+      <c r="D3" s="117"/>
+      <c r="E3" s="117"/>
+      <c r="F3" s="117"/>
+      <c r="G3" s="117"/>
+      <c r="H3" s="117"/>
+      <c r="K3" s="147"/>
+      <c r="L3" s="148"/>
+      <c r="M3" s="148"/>
+      <c r="N3" s="148"/>
       <c r="O3" s="80"/>
     </row>
     <row r="4" spans="1:15">
@@ -4104,11 +4100,11 @@
       <c r="A2" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="B2" s="150" t="s">
+      <c r="B2" s="151" t="s">
         <v>99</v>
       </c>
-      <c r="C2" s="123"/>
-      <c r="D2" s="123"/>
+      <c r="C2" s="117"/>
+      <c r="D2" s="117"/>
       <c r="G2" s="4"/>
       <c r="H2" s="1" t="s">
         <v>100</v>
@@ -4170,11 +4166,11 @@
       <c r="T4" s="4"/>
     </row>
     <row r="5" spans="1:20" ht="184.8">
-      <c r="B5" s="148" t="s">
+      <c r="B5" s="149" t="s">
         <v>106</v>
       </c>
-      <c r="C5" s="123"/>
-      <c r="D5" s="123"/>
+      <c r="C5" s="117"/>
+      <c r="D5" s="117"/>
       <c r="F5" s="10">
         <v>6.1</v>
       </c>
@@ -4257,11 +4253,11 @@
       <c r="T6" s="4"/>
     </row>
     <row r="7" spans="1:20" ht="79.8">
-      <c r="B7" s="148" t="s">
+      <c r="B7" s="149" t="s">
         <v>120</v>
       </c>
-      <c r="C7" s="123"/>
-      <c r="D7" s="123"/>
+      <c r="C7" s="117"/>
+      <c r="D7" s="117"/>
       <c r="F7" s="10">
         <v>6.2</v>
       </c>
@@ -4313,11 +4309,11 @@
       <c r="T7" s="2"/>
     </row>
     <row r="8" spans="1:20" ht="66.599999999999994">
-      <c r="B8" s="148" t="s">
+      <c r="B8" s="149" t="s">
         <v>128</v>
       </c>
-      <c r="C8" s="123"/>
-      <c r="D8" s="123"/>
+      <c r="C8" s="117"/>
+      <c r="D8" s="117"/>
       <c r="G8" s="4"/>
       <c r="H8" s="9" t="s">
         <v>114</v>
@@ -4381,9 +4377,9 @@
       <c r="M12" s="11"/>
     </row>
     <row r="13" spans="1:20" ht="13.8">
-      <c r="B13" s="149"/>
-      <c r="C13" s="123"/>
-      <c r="D13" s="123"/>
+      <c r="B13" s="150"/>
+      <c r="C13" s="117"/>
+      <c r="D13" s="117"/>
       <c r="G13" s="10"/>
       <c r="H13" s="4" t="s">
         <v>134</v>
@@ -4405,11 +4401,11 @@
       </c>
     </row>
     <row r="14" spans="1:20" ht="70.5" customHeight="1">
-      <c r="B14" s="148" t="s">
+      <c r="B14" s="149" t="s">
         <v>140</v>
       </c>
-      <c r="C14" s="123"/>
-      <c r="D14" s="123"/>
+      <c r="C14" s="117"/>
+      <c r="D14" s="117"/>
       <c r="F14" s="10">
         <v>3.1</v>
       </c>
@@ -4500,11 +4496,11 @@
       <c r="M17" s="4"/>
     </row>
     <row r="18" spans="2:19" ht="251.4">
-      <c r="B18" s="148" t="s">
+      <c r="B18" s="149" t="s">
         <v>152</v>
       </c>
-      <c r="C18" s="123"/>
-      <c r="D18" s="123"/>
+      <c r="C18" s="117"/>
+      <c r="D18" s="117"/>
       <c r="F18" s="10">
         <v>3.2</v>
       </c>
@@ -4615,11 +4611,11 @@
       </c>
     </row>
     <row r="25" spans="2:19" ht="290.39999999999998">
-      <c r="B25" s="149" t="s">
+      <c r="B25" s="150" t="s">
         <v>164</v>
       </c>
-      <c r="C25" s="123"/>
-      <c r="D25" s="123"/>
+      <c r="C25" s="117"/>
+      <c r="D25" s="117"/>
       <c r="G25" s="10" t="s">
         <v>165</v>
       </c>
@@ -4664,9 +4660,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4885,27 +4884,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3D98D897-3D5D-4CF5-A274-8B2E15AE73B2}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3BB72468-B9EB-412A-8D55-6151E9A308C0}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="bd38d267-56bb-4e22-b975-199a06fd69fa"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="d8c712e5-67fc-4595-93cb-a4164dd8eff3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -4930,9 +4917,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3BB72468-B9EB-412A-8D55-6151E9A308C0}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3D98D897-3D5D-4CF5-A274-8B2E15AE73B2}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="bd38d267-56bb-4e22-b975-199a06fd69fa"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="d8c712e5-67fc-4595-93cb-a4164dd8eff3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>